<commit_message>
add column link for table product - API user fix exception
</commit_message>
<xml_diff>
--- a/src/main/resources/db/scripts/data/product.xlsx
+++ b/src/main/resources/db/scripts/data/product.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\My-Project\voluongquang\be-voluongquang\src\main\resources\db\scripts\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D38C2A8E-BC7B-4551-979C-66CC98300063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0EB7601-80DB-4EE7-97E3-295A1624ECED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{561D3704-9A42-4F37-A12C-2F4276FAE1F4}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1887" uniqueCount="967">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1888" uniqueCount="968">
   <si>
     <t>product_id</t>
   </si>
@@ -2921,6 +2921,9 @@
   </si>
   <si>
     <t>Hủ tíu nam vang âu lạc</t>
+  </si>
+  <si>
+    <t>link</t>
   </si>
 </sst>
 </file>
@@ -3781,13 +3784,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{391DB971-0CAD-414C-BD50-8AC205D98293}">
-  <dimension ref="A1:R432"/>
+  <dimension ref="A1:S432"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3837,13 +3842,16 @@
         <v>15</v>
       </c>
       <c r="Q1" t="s">
+        <v>967</v>
+      </c>
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -3860,7 +3868,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -3880,7 +3888,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -3897,7 +3905,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -3914,7 +3922,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -3931,7 +3939,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -3951,7 +3959,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -3971,7 +3979,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -3991,7 +3999,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -4008,7 +4016,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -4025,7 +4033,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -4045,7 +4053,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>47</v>
       </c>
@@ -4065,7 +4073,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -4082,7 +4090,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -4099,7 +4107,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>56</v>
       </c>

</xml_diff>